<commit_message>
Fixed spelling mistakes on the checklist documents
</commit_message>
<xml_diff>
--- a/documents/cypress_eh_qrda_category_1_validation_checklist_04262013.xlsx
+++ b/documents/cypress_eh_qrda_category_1_validation_checklist_04262013.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3600" yWindow="840" windowWidth="24375" windowHeight="18240" tabRatio="969"/>
+    <workbookView xWindow="3600" yWindow="840" windowWidth="24375" windowHeight="18240" tabRatio="969" firstSheet="31" activeTab="55"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="56" r:id="rId1"/>
@@ -676,7 +676,6 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Verdana"/>
-        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -687,36 +686,6 @@
         <family val="2"/>
       </rPr>
       <t>For each Template ID found in the QRDA Category 1 XML, you should then identify the proper "Value Set OID" associated with each "Template ID" in the QRDA Category 1 XML.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Step 1: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-      </rPr>
-      <t>Identify which CQM you performed the QRDA Category 1 XML "Capture and Export" test.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-      </rPr>
-      <t>You will need to ensure that the CQM that you are testing for QRDA Category 1 XML testing for a "Capture and Export" test maps to the CQMs enumerated to the Cypress QRDA Category 1 Validation Checklist.  The CQM identifier is available via the Cypress "Product" page, in the name of the tests enumerated on that Cypress page.</t>
     </r>
   </si>
   <si>
@@ -752,7 +721,37 @@
         <rFont val="Verdana"/>
         <family val="2"/>
       </rPr>
-      <t>The patient names generated by Cypress are randomly assigned to the records before they are presented from Cypress to an EHR system.  In order to translate the  short-hand names that are provided in this Cypress QRDA Category 1 Validation Checklist document, you will need to identify the "Name" from the data presented by the EHR associated with the QRDA Category 1 XML</t>
+      <t>The patient names generated by Cypress are randomly assigned to the records before they are presented from Cypress to an EHR system.  In order to translate the  short-hand names that are provide in this Cypress QRDA Category 1 Validation Checklist document, you will need to identify the "Name" from the data presented by the EHR associated with the QRDA Category 1 XML</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Step 1: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t>Identify which CQM you performed the QRDA Category 1 XML "Capture and Export" test.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t>You will need to ensure that the CQM that you are testing for QRDA Category 1 XML testing for a "Capture and Export" test maps to the CQMs enumerated to the Cypress QRDA Category 1 Validation Checklist.  The CQM identifier is available via the Cypress "Product" page, in the name of the tests enumerated on that Cypress page.</t>
     </r>
   </si>
 </sst>
@@ -1591,8 +1590,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1617,7 +1616,7 @@
     </row>
     <row r="4" spans="1:1" ht="70.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="134.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -1625,7 +1624,7 @@
     </row>
     <row r="6" spans="1:1" ht="81" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="162.94999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -1678,14 +1677,14 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="38.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -2110,9 +2109,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="40.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -2384,9 +2384,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="51.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="58.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -2627,14 +2628,15 @@
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="42.75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -2900,9 +2902,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="41.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -3064,10 +3067,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -3247,14 +3250,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -3456,14 +3461,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -3647,10 +3654,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -3863,14 +3870,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D56" sqref="D56"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="51.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="58.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -4034,9 +4043,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="46" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -4236,10 +4246,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -4401,10 +4411,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="98.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="114.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -4962,9 +4972,9 @@
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -5132,10 +5142,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -5281,10 +5291,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -5426,14 +5436,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -5812,9 +5824,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.75" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5907,9 +5919,9 @@
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -6322,10 +6334,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="46" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -6434,9 +6446,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="62.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="72.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -6593,10 +6606,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="46" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -6773,10 +6786,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="46" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -6883,10 +6896,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="44.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -7276,10 +7289,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="44.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -7382,8 +7395,8 @@
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="44.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.75" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -7808,10 +7821,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="54.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="62.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -8309,14 +8322,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -8785,9 +8800,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="36.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -8896,14 +8912,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -9373,9 +9391,9 @@
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -9846,9 +9864,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="32.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -10320,8 +10339,8 @@
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -10787,14 +10806,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -11259,14 +11280,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0"/>
+    <sheetView topLeftCell="C3" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -11737,8 +11758,8 @@
   <cols>
     <col min="1" max="1" width="14.625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="98.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -12284,10 +12305,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="98.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -12796,7 +12817,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C56" sqref="C56"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -13320,8 +13343,8 @@
   <cols>
     <col min="1" max="1" width="14.625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="98.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -13834,9 +13857,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="46" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -14071,8 +14095,8 @@
   <cols>
     <col min="1" max="1" width="14.625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="98.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -14587,8 +14611,8 @@
   <cols>
     <col min="1" max="1" width="14.625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="98.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -15105,8 +15129,8 @@
   <cols>
     <col min="1" max="1" width="14.625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="98.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -15621,8 +15645,8 @@
   <cols>
     <col min="1" max="1" width="14.625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="98.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -16474,16 +16498,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -16658,9 +16682,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="48.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="56.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -17060,14 +17085,14 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="51.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="58.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -17363,10 +17388,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -17963,10 +17988,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>